<commit_message>
final update S2 main study
</commit_message>
<xml_diff>
--- a/Studies/S2_softRobots/t2_CAMs/post_CAMsecond/static/Scale Heerink et al., 2010/items Heerink 2010.xlsx
+++ b/Studies/S2_softRobots/t2_CAMs/post_CAMsecond/static/Scale Heerink et al., 2010/items Heerink 2010.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\DATEN\PHD\labjsSoftware\livmats studies\Studies\S2_softRobots\t2_CAMs\post_CAMsecond\static\Scale Heerink et al., 2010\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\DATEN\PHD\JATOSSoftware\study_assets_root\S2_CAMstudy\post_CAMsecond\static\Scale Heerink et al., 2010\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:81_{0321A9F3-88B4-4F53-8BE4-A24E6AC86F6B}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:81_{FEA6839B-70EA-42A0-B82D-A61124C5A4E6}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-105" yWindow="-105" windowWidth="23250" windowHeight="12570" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -18,8 +18,8 @@
   <calcPr calcId="191029"/>
   <customWorkbookViews>
     <customWorkbookView name="Julius Fenn - Persönliche Ansicht" guid="{0AB4E75F-2D7B-4C5A-AD7C-1837EAFF8F53}" mergeInterval="0" personalView="1" maximized="1" xWindow="1912" yWindow="-8" windowWidth="2576" windowHeight="1416" activeSheetId="1"/>
+    <customWorkbookView name="Microsoft Office-Anwender - Persönliche Ansicht" guid="{890A2A41-DF1E-FA42-8D9E-8E3DE3754670}" mergeInterval="0" personalView="1" windowWidth="1365" windowHeight="704" activeSheetId="1"/>
     <customWorkbookView name="Philipp Höfele - Persönliche Ansicht" guid="{47B4CD57-5B2E-4389-ABE6-89250A82D1C8}" mergeInterval="0" personalView="1" maximized="1" xWindow="-9" yWindow="-9" windowWidth="1938" windowHeight="1048" activeSheetId="1"/>
-    <customWorkbookView name="Microsoft Office-Anwender - Persönliche Ansicht" guid="{890A2A41-DF1E-FA42-8D9E-8E3DE3754670}" mergeInterval="0" personalView="1" windowWidth="1365" windowHeight="704" activeSheetId="1"/>
   </customWorkbookViews>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
@@ -77,13 +77,13 @@
     <t>Ich finde den Roboter einschüchternd.</t>
   </si>
   <si>
-    <t>Ich denke es ist eine gute Idee den Roboter zu verwenden.</t>
-  </si>
-  <si>
     <t>Der Roboter würde das Leben Interessanter machen.</t>
   </si>
   <si>
     <t>Es ist gut, einen Nutzen aus dem Roboter zu ziehen.</t>
+  </si>
+  <si>
+    <t>Ich denke es ist eine gute Idee, den Roboter zu verwenden.</t>
   </si>
 </sst>
 </file>
@@ -146,7 +146,7 @@
 </file>
 
 <file path=xl/revisions/revisionHeaders.xml><?xml version="1.0" encoding="utf-8"?>
-<headers xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac" guid="{D28ECF1C-E941-4ED1-9462-1BB6AA66429E}" diskRevisions="1" revisionId="1051" version="37">
+<headers xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac" guid="{1FD10D72-309E-45D9-8183-4C09068931E3}" diskRevisions="1" revisionId="1052" version="38">
   <header guid="{09193A18-0B52-4FAB-B338-B4D967DC2D75}" dateTime="2022-09-29T13:56:20" maxSheetId="2" userName="Julius Fenn" r:id="rId23" minRId="265" maxRId="270">
     <sheetIdMap count="1">
       <sheetId val="1"/>
@@ -237,6 +237,11 @@
       <sheetId val="1"/>
     </sheetIdMap>
   </header>
+  <header guid="{1FD10D72-309E-45D9-8183-4C09068931E3}" dateTime="2023-12-11T08:58:38" maxSheetId="2" userName="Julius Fenn" r:id="rId41" minRId="1052">
+    <sheetIdMap count="1">
+      <sheetId val="1"/>
+    </sheetIdMap>
+  </header>
 </headers>
 </file>
 
@@ -3781,6 +3786,25 @@
       <alignment wrapText="1"/>
     </dxf>
   </rfmt>
+</revisions>
+</file>
+
+<file path=xl/revisions/revisionLog11.xml><?xml version="1.0" encoding="utf-8"?>
+<revisions xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <rcc rId="1052" sId="1">
+    <oc r="B6" t="inlineStr">
+      <is>
+        <t>Ich denke es ist eine gute Idee den Roboter zu verwenden.</t>
+      </is>
+    </oc>
+    <nc r="B6" t="inlineStr">
+      <is>
+        <t>Ich denke es ist eine gute Idee, den Roboter zu verwenden.</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcv guid="{0AB4E75F-2D7B-4C5A-AD7C-1837EAFF8F53}" action="delete"/>
+  <rcv guid="{0AB4E75F-2D7B-4C5A-AD7C-1837EAFF8F53}" action="add"/>
 </revisions>
 </file>
 
@@ -15240,7 +15264,7 @@
   <dimension ref="A1:B8"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="190" zoomScaleNormal="190" workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
+      <selection activeCell="B19" sqref="B19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -15295,7 +15319,7 @@
         <v>6</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
@@ -15303,7 +15327,7 @@
         <v>7</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
@@ -15311,23 +15335,23 @@
         <v>8</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
   </sheetData>
   <customSheetViews>
     <customSheetView guid="{0AB4E75F-2D7B-4C5A-AD7C-1837EAFF8F53}" scale="190" showPageBreaks="1" fitToPage="1">
-      <selection activeCell="B12" sqref="B12"/>
+      <selection activeCell="B19" sqref="B19"/>
       <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
       <pageSetup paperSize="9" fitToHeight="0" orientation="portrait" r:id="rId1"/>
     </customSheetView>
-    <customSheetView guid="{47B4CD57-5B2E-4389-ABE6-89250A82D1C8}" scale="90" topLeftCell="B40">
-      <selection activeCell="F45" sqref="F45"/>
+    <customSheetView guid="{890A2A41-DF1E-FA42-8D9E-8E3DE3754670}" scale="133" topLeftCell="A10">
+      <selection activeCell="E18" sqref="E18"/>
       <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
       <pageSetup paperSize="9" orientation="portrait" r:id="rId2"/>
     </customSheetView>
-    <customSheetView guid="{890A2A41-DF1E-FA42-8D9E-8E3DE3754670}" scale="133" topLeftCell="A10">
-      <selection activeCell="E18" sqref="E18"/>
+    <customSheetView guid="{47B4CD57-5B2E-4389-ABE6-89250A82D1C8}" scale="90" topLeftCell="B40">
+      <selection activeCell="F45" sqref="F45"/>
       <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
       <pageSetup paperSize="9" orientation="portrait" r:id="rId3"/>
     </customSheetView>

</xml_diff>